<commit_message>
Changes to eval_results to evaluate with results with prompting
Also updates results.xlsx with prompt_id 1 run details.
</commit_message>
<xml_diff>
--- a/results/mbpp/results.xlsx
+++ b/results/mbpp/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anoop\Academics\ASU\Semester 1\CSE 576\Projects\Quirky_Quartet\results\mbpp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshit/Documents/GitHub/Quirky_Quartet/results/mbpp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B4A6E8B-D4DE-4DF6-A19F-C74E5F77B072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA1B420-1F15-A846-BC55-1B2CC9257B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3DDA5BEF-13D0-4759-96E3-91280D99A532}"/>
+    <workbookView xWindow="-34940" yWindow="3880" windowWidth="25680" windowHeight="14900" xr2:uid="{3DDA5BEF-13D0-4759-96E3-91280D99A532}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="17">
   <si>
     <t>Setting</t>
   </si>
@@ -75,13 +78,22 @@
   </si>
   <si>
     <t>Total Unparseable</t>
+  </si>
+  <si>
+    <t>Prompt_id 1 - Results pass @ 5</t>
+  </si>
+  <si>
+    <t>Prompt_id 1 - Results pass @ 1</t>
+  </si>
+  <si>
+    <t>Prompt_id 1 - Results pass @ 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,13 +116,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -126,20 +150,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -451,65 +483,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F64B8FC-649F-4A60-B32B-397739CC3A95}">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -522,19 +554,19 @@
       <c r="D3">
         <v>89</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <f>B3/SUM(B3:D3)</f>
         <v>5.9405940594059403E-2</v>
       </c>
       <c r="F3">
         <v>89</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="2">
         <f>F3/SUM(B3:D3)</f>
         <v>0.88118811881188119</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -547,44 +579,44 @@
       <c r="D4">
         <v>70</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <f>B4/SUM(B4:D4)</f>
         <v>9.9009900990099015E-2</v>
       </c>
       <c r="F4">
         <v>70</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="2">
         <f>F4/SUM(B4:D4)</f>
         <v>0.69306930693069302</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="7">
         <v>16</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="7">
         <v>35</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="7">
         <v>50</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="8">
         <f t="shared" ref="E5:E6" si="0">B5/SUM(B5:D5)</f>
         <v>0.15841584158415842</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="7">
         <v>50</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="8">
         <f t="shared" ref="G5:G6" si="1">F5/SUM(B5:D5)</f>
         <v>0.49504950495049505</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -597,53 +629,53 @@
       <c r="D6">
         <v>55</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>0.10891089108910891</v>
       </c>
       <c r="F6">
         <v>55</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="2">
         <f t="shared" si="1"/>
         <v>0.54455445544554459</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -656,19 +688,19 @@
       <c r="D10">
         <v>77</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="2">
         <f>B10/SUM(B10:D10)</f>
         <v>9.9009900990099015E-2</v>
       </c>
       <c r="F10">
         <v>176</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="2">
         <f>F10/(SUM(B10:D10)*2)</f>
         <v>0.87128712871287128</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -681,44 +713,44 @@
       <c r="D11">
         <v>49</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="2">
         <f>B11/SUM(B11:D11)</f>
         <v>0.17821782178217821</v>
       </c>
       <c r="F11">
         <v>138</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="2">
         <f>F11/(SUM(B11:D11)*2)</f>
         <v>0.68316831683168322</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="12" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="7">
         <v>24</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="7">
         <v>51</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="7">
         <v>26</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="8">
         <f t="shared" ref="E12:E13" si="2">B12/SUM(B12:D12)</f>
         <v>0.23762376237623761</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="7">
         <v>103</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="8">
         <f t="shared" ref="G12:G13" si="3">F12/(SUM(B12:D12)*2)</f>
         <v>0.50990099009900991</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -731,53 +763,53 @@
       <c r="D13">
         <v>30</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="2">
         <f t="shared" si="2"/>
         <v>0.21782178217821782</v>
       </c>
       <c r="F13">
         <v>111</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="2">
         <f t="shared" si="3"/>
         <v>0.54950495049504955</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -790,19 +822,19 @@
       <c r="D17">
         <v>42</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="2">
         <f>B17/SUM(B17:D17)</f>
         <v>0.21782178217821782</v>
       </c>
       <c r="F17">
         <v>426</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="2">
         <f>F17/(SUM(B17:D17)*5)</f>
         <v>0.84356435643564354</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -815,44 +847,44 @@
       <c r="D18">
         <v>20</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="2">
         <f t="shared" ref="E18:E20" si="4">B18/SUM(B18:D18)</f>
         <v>0.28712871287128711</v>
       </c>
       <c r="F18">
         <v>331</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="2">
         <f t="shared" ref="G18:G20" si="5">F18/(SUM(B18:D18)*5)</f>
         <v>0.65544554455445547</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="7">
         <v>38</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="7">
         <v>54</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="7">
         <v>9</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="8">
         <f t="shared" si="4"/>
         <v>0.37623762376237624</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="7">
         <v>268</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="8">
         <f t="shared" si="5"/>
         <v>0.53069306930693072</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -865,16 +897,181 @@
       <c r="D20">
         <v>5</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="2">
         <f t="shared" si="4"/>
         <v>0.38613861386138615</v>
       </c>
       <c r="F20">
         <v>259</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="2">
         <f t="shared" si="5"/>
         <v>0.51287128712871288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="7">
+        <v>13</v>
+      </c>
+      <c r="C24" s="7">
+        <v>35</v>
+      </c>
+      <c r="D24" s="7">
+        <v>55</v>
+      </c>
+      <c r="E24" s="8">
+        <f>B24/SUM(B24:D24)</f>
+        <v>0.12621359223300971</v>
+      </c>
+      <c r="F24" s="7">
+        <v>55</v>
+      </c>
+      <c r="G24" s="8">
+        <f>F24/(SUM(B24:D24)*5)</f>
+        <v>0.10679611650485436</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="7">
+        <v>22</v>
+      </c>
+      <c r="C28" s="7">
+        <v>46</v>
+      </c>
+      <c r="D28" s="7">
+        <v>35</v>
+      </c>
+      <c r="E28" s="8">
+        <f>B28/SUM(B28:D28)</f>
+        <v>0.21359223300970873</v>
+      </c>
+      <c r="F28" s="7">
+        <v>115</v>
+      </c>
+      <c r="G28" s="8">
+        <f>F28/(SUM(B28:D28)*5)</f>
+        <v>0.22330097087378642</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="7">
+        <v>43</v>
+      </c>
+      <c r="C32" s="7">
+        <v>53</v>
+      </c>
+      <c r="D32" s="7">
+        <v>7</v>
+      </c>
+      <c r="E32" s="8">
+        <f>B32/SUM(B32:D32)</f>
+        <v>0.41747572815533979</v>
+      </c>
+      <c r="F32" s="7">
+        <v>274</v>
+      </c>
+      <c r="G32" s="8">
+        <f>F32/(SUM(B32:D32)*5)</f>
+        <v>0.53203883495145632</v>
       </c>
     </row>
   </sheetData>
@@ -885,6 +1082,7 @@
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A15:G15"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated results for MBPP with prompt 0 in 5-shot setting
</commit_message>
<xml_diff>
--- a/results/mbpp/results.xlsx
+++ b/results/mbpp/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshit/Documents/GitHub/Quirky_Quartet/results/mbpp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anoop\Academics\ASU\Semester 1\CSE 576\Projects\Quirky_Quartet\results\mbpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA1B420-1F15-A846-BC55-1B2CC9257B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471D7B0C-87ED-4D4B-8931-3D92B79890BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34940" yWindow="3880" windowWidth="25680" windowHeight="14900" xr2:uid="{3DDA5BEF-13D0-4759-96E3-91280D99A532}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3DDA5BEF-13D0-4759-96E3-91280D99A532}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="26">
   <si>
     <t>Setting</t>
   </si>
@@ -80,13 +77,40 @@
     <t>Total Unparseable</t>
   </si>
   <si>
-    <t>Prompt_id 1 - Results pass @ 5</t>
-  </si>
-  <si>
-    <t>Prompt_id 1 - Results pass @ 1</t>
-  </si>
-  <si>
-    <t>Prompt_id 1 - Results pass @ 2</t>
+    <t>Prompt_id 0 - Results @ 1</t>
+  </si>
+  <si>
+    <t>Prompt_id 0 - Results @ 2</t>
+  </si>
+  <si>
+    <t>Prompt_id 0 - Results @ 5</t>
+  </si>
+  <si>
+    <t>Prompt_id 1 - Results @ 1</t>
+  </si>
+  <si>
+    <t>Prompt_id 1 - Results @ 2</t>
+  </si>
+  <si>
+    <t>Prompt_id 1 - Results @ 5</t>
+  </si>
+  <si>
+    <t>Prompt_id 2 - Results @ 1</t>
+  </si>
+  <si>
+    <t>Prompt_id 2 - Results @ 2</t>
+  </si>
+  <si>
+    <t>Prompt_id 2 - Results @ 5</t>
+  </si>
+  <si>
+    <t>Prompt_id 3 - Results @ 1</t>
+  </si>
+  <si>
+    <t>Prompt_id 3 - Results @ 2</t>
+  </si>
+  <si>
+    <t>Prompt_id 3 - Results @ 5</t>
   </si>
 </sst>
 </file>
@@ -123,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +157,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,28 +180,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -483,42 +513,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F64B8FC-649F-4A60-B32B-397739CC3A95}">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90:G90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,7 +571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -566,7 +596,7 @@
         <v>0.88118811881188119</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -591,32 +621,32 @@
         <v>0.69306930693069302</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="3">
         <v>16</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="3">
         <v>35</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="3">
         <v>50</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="4">
         <f t="shared" ref="E5:E6" si="0">B5/SUM(B5:D5)</f>
         <v>0.15841584158415842</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="3">
         <v>50</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="4">
         <f t="shared" ref="G5:G6" si="1">F5/SUM(B5:D5)</f>
         <v>0.49504950495049505</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -641,18 +671,18 @@
         <v>0.54455445544554459</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,7 +705,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -700,7 +730,7 @@
         <v>0.87128712871287128</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -725,32 +755,32 @@
         <v>0.68316831683168322</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="3">
         <v>24</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="3">
         <v>51</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="3">
         <v>26</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="4">
         <f t="shared" ref="E12:E13" si="2">B12/SUM(B12:D12)</f>
         <v>0.23762376237623761</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="3">
         <v>103</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="4">
         <f t="shared" ref="G12:G13" si="3">F12/(SUM(B12:D12)*2)</f>
         <v>0.50990099009900991</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -775,18 +805,18 @@
         <v>0.54950495049504955</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -809,7 +839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -834,7 +864,7 @@
         <v>0.84356435643564354</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -859,32 +889,32 @@
         <v>0.65544554455445547</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="3">
         <v>38</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="3">
         <v>54</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="3">
         <v>9</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="4">
         <f t="shared" si="4"/>
         <v>0.37623762376237624</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="3">
         <v>268</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="4">
         <f t="shared" si="5"/>
         <v>0.53069306930693072</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -909,175 +939,825 @@
         <v>0.51287128712871288</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D22" s="6" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="3">
+        <v>19</v>
+      </c>
+      <c r="C27" s="3">
+        <v>32</v>
+      </c>
+      <c r="D27" s="3">
+        <v>50</v>
+      </c>
+      <c r="E27" s="4">
+        <f>B27/SUM(B27:D27)</f>
+        <v>0.18811881188118812</v>
+      </c>
+      <c r="F27" s="3">
+        <v>50</v>
+      </c>
+      <c r="G27" s="4">
+        <f>F27/(SUM(B27:D27)*1)</f>
+        <v>0.49504950495049505</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B32" s="3">
+        <v>25</v>
+      </c>
+      <c r="C32" s="3">
+        <v>49</v>
+      </c>
+      <c r="D32" s="3">
+        <v>27</v>
+      </c>
+      <c r="E32" s="4">
+        <f>B32/SUM(B32:D32)</f>
+        <v>0.24752475247524752</v>
+      </c>
+      <c r="F32" s="3">
+        <v>105</v>
+      </c>
+      <c r="G32" s="4">
+        <f>F32/(SUM(B32:D32)*2)</f>
+        <v>0.51980198019801982</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="7">
+      <c r="G35" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="3">
+        <v>43</v>
+      </c>
+      <c r="C37" s="3">
+        <v>51</v>
+      </c>
+      <c r="D37" s="3">
+        <v>7</v>
+      </c>
+      <c r="E37" s="4">
+        <f>B37/SUM(B37:D37)</f>
+        <v>0.42574257425742573</v>
+      </c>
+      <c r="F37" s="3">
+        <v>259</v>
+      </c>
+      <c r="G37" s="4">
+        <f>F37/(SUM(B37:D37)*5)</f>
+        <v>0.51287128712871288</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="7"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="3">
+        <v>13</v>
+      </c>
+      <c r="C44" s="3">
         <v>35</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D44" s="3">
         <v>55</v>
       </c>
-      <c r="E24" s="8">
-        <f>B24/SUM(B24:D24)</f>
+      <c r="E44" s="4">
+        <f>B44/SUM(B44:D44)</f>
         <v>0.12621359223300971</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F44" s="3">
         <v>55</v>
       </c>
-      <c r="G24" s="8">
-        <f>F24/(SUM(B24:D24)*5)</f>
-        <v>0.10679611650485436</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="G44" s="4">
+        <f>F44/(SUM(B44:D44)*1)</f>
+        <v>0.53398058252427183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B49" s="3">
         <v>22</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C49" s="3">
         <v>46</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D49" s="3">
         <v>35</v>
       </c>
-      <c r="E28" s="8">
-        <f>B28/SUM(B28:D28)</f>
+      <c r="E49" s="4">
+        <f>B49/SUM(B49:D49)</f>
         <v>0.21359223300970873</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F49" s="3">
         <v>115</v>
       </c>
-      <c r="G28" s="8">
-        <f>F28/(SUM(B28:D28)*5)</f>
-        <v>0.22330097087378642</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D30" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="G49" s="4">
+        <f>F49/(SUM(B49:D49)*2)</f>
+        <v>0.55825242718446599</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B54" s="3">
         <v>43</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C54" s="3">
         <v>53</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D54" s="3">
         <v>7</v>
       </c>
-      <c r="E32" s="8">
-        <f>B32/SUM(B32:D32)</f>
+      <c r="E54" s="4">
+        <f>B54/SUM(B54:D54)</f>
         <v>0.41747572815533979</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F54" s="3">
         <v>274</v>
       </c>
-      <c r="G32" s="8">
-        <f>F32/(SUM(B32:D32)*5)</f>
+      <c r="G54" s="4">
+        <f>F54/(SUM(B54:D54)*5)</f>
         <v>0.53203883495145632</v>
       </c>
     </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="7"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="4"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="7"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="4"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A70" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="7"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A71" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="4"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A73" s="10"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="7"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A78" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="4"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" s="9"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="7"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="4"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B85" s="9"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="7"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="4"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="10"/>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:Q1"/>
+  <mergeCells count="15">
+    <mergeCell ref="A80:G80"/>
+    <mergeCell ref="A85:G85"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="A58:G58"/>
+    <mergeCell ref="A63:G63"/>
+    <mergeCell ref="A68:G68"/>
+    <mergeCell ref="A75:G75"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="A46:G46"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A15:G15"/>

</xml_diff>

<commit_message>
Updated results for MBPP with prompt 2 in 5-shot setting
</commit_message>
<xml_diff>
--- a/results/mbpp/results.xlsx
+++ b/results/mbpp/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anoop\Academics\ASU\Semester 1\CSE 576\Projects\Quirky_Quartet\results\mbpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471D7B0C-87ED-4D4B-8931-3D92B79890BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6E0089-1DFA-4058-8EE9-30F3363E651B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3DDA5BEF-13D0-4759-96E3-91280D99A532}"/>
   </bookViews>
@@ -180,24 +180,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F64B8FC-649F-4A60-B32B-397739CC3A95}">
-  <dimension ref="A1:Q90"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90:G90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -527,28 +525,18 @@
     <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,7 +559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -596,7 +584,7 @@
         <v>0.88118811881188119</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -621,7 +609,7 @@
         <v>0.69306930693069302</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -646,7 +634,7 @@
         <v>0.49504950495049505</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -671,18 +659,18 @@
         <v>0.54455445544554459</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,7 +693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -730,7 +718,7 @@
         <v>0.87128712871287128</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -755,7 +743,7 @@
         <v>0.68316831683168322</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -780,7 +768,7 @@
         <v>0.50990099009900991</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -805,18 +793,18 @@
         <v>0.54950495049504955</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -889,7 +877,7 @@
         <v>0.65544554455445547</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
@@ -944,24 +932,24 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="11"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
@@ -987,17 +975,13 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
+      <c r="A26" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>3</v>
       </c>
@@ -1023,15 +1007,15 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
@@ -1057,17 +1041,13 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
+      <c r="A31" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>3</v>
       </c>
@@ -1093,15 +1073,15 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -1127,17 +1107,13 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="6" t="s">
+      <c r="A36" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E36" s="5"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>3</v>
       </c>
@@ -1163,24 +1139,24 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
@@ -1206,15 +1182,11 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="6" t="s">
+      <c r="A43" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="7"/>
+      <c r="E43" s="5"/>
+      <c r="G43" s="5"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
@@ -1242,15 +1214,15 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
@@ -1276,15 +1248,11 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="6" t="s">
+      <c r="A48" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="7"/>
+      <c r="E48" s="5"/>
+      <c r="G48" s="5"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
@@ -1312,15 +1280,15 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
@@ -1346,15 +1314,11 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="6" t="s">
+      <c r="A53" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="7"/>
+      <c r="E53" s="5"/>
+      <c r="G53" s="5"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
@@ -1382,24 +1346,24 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
@@ -1425,37 +1389,47 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" s="6" t="s">
+      <c r="A60" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="6"/>
-      <c r="G60" s="7"/>
+      <c r="E60" s="5"/>
+      <c r="G60" s="5"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="4"/>
+      <c r="B61" s="3">
+        <v>15</v>
+      </c>
+      <c r="C61" s="3">
+        <v>30</v>
+      </c>
+      <c r="D61" s="3">
+        <v>56</v>
+      </c>
+      <c r="E61" s="4">
+        <f>B61/SUM(B61:D61)</f>
+        <v>0.14851485148514851</v>
+      </c>
+      <c r="F61" s="3">
+        <v>56</v>
+      </c>
+      <c r="G61" s="4">
+        <f>F61/(SUM(B61:D61)*1)</f>
+        <v>0.5544554455445545</v>
+      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B63" s="9"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
@@ -1481,37 +1455,47 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="6" t="s">
+      <c r="A65" t="s">
         <v>1</v>
       </c>
-      <c r="B65" s="6"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="6"/>
-      <c r="G65" s="7"/>
+      <c r="E65" s="5"/>
+      <c r="G65" s="5"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="4"/>
+      <c r="B66" s="3">
+        <v>26</v>
+      </c>
+      <c r="C66" s="3">
+        <v>47</v>
+      </c>
+      <c r="D66" s="3">
+        <v>28</v>
+      </c>
+      <c r="E66" s="4">
+        <f>B66/SUM(B66:D66)</f>
+        <v>0.25742574257425743</v>
+      </c>
+      <c r="F66" s="3">
+        <v>114</v>
+      </c>
+      <c r="G66" s="4">
+        <f>F66/(SUM(B66:D66)*2)</f>
+        <v>0.5643564356435643</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" s="9" t="s">
+      <c r="A68" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
@@ -1537,46 +1521,56 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" s="6" t="s">
+      <c r="A70" t="s">
         <v>1</v>
       </c>
-      <c r="B70" s="6"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="6"/>
-      <c r="G70" s="7"/>
+      <c r="E70" s="5"/>
+      <c r="G70" s="5"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="4"/>
+      <c r="B71" s="3">
+        <v>44</v>
+      </c>
+      <c r="C71" s="3">
+        <v>54</v>
+      </c>
+      <c r="D71" s="3">
+        <v>3</v>
+      </c>
+      <c r="E71" s="4">
+        <f>B71/SUM(B71:D71)</f>
+        <v>0.43564356435643564</v>
+      </c>
+      <c r="F71" s="3">
+        <v>258</v>
+      </c>
+      <c r="G71" s="4">
+        <f>F71/(SUM(B71:D71)*5)</f>
+        <v>0.5108910891089109</v>
+      </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73" s="10"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="10"/>
-      <c r="G73" s="10"/>
+      <c r="A73" s="6"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" s="9" t="s">
+      <c r="A75" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B75" s="9"/>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9"/>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9"/>
-      <c r="G75" s="9"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="8"/>
+      <c r="G75" s="8"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
@@ -1602,15 +1596,11 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A77" s="6" t="s">
+      <c r="A77" t="s">
         <v>1</v>
       </c>
-      <c r="B77" s="6"/>
-      <c r="C77" s="6"/>
-      <c r="D77" s="6"/>
-      <c r="E77" s="7"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="7"/>
+      <c r="E77" s="5"/>
+      <c r="G77" s="5"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
@@ -1624,15 +1614,15 @@
       <c r="G78" s="4"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" s="9" t="s">
+      <c r="A80" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B80" s="9"/>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+      <c r="G80" s="8"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
@@ -1658,15 +1648,11 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82" s="6" t="s">
+      <c r="A82" t="s">
         <v>1</v>
       </c>
-      <c r="B82" s="6"/>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="6"/>
-      <c r="G82" s="7"/>
+      <c r="E82" s="5"/>
+      <c r="G82" s="5"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
@@ -1680,15 +1666,15 @@
       <c r="G83" s="4"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A85" s="9" t="s">
+      <c r="A85" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B85" s="9"/>
-      <c r="C85" s="9"/>
-      <c r="D85" s="9"/>
-      <c r="E85" s="9"/>
-      <c r="F85" s="9"/>
-      <c r="G85" s="9"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
@@ -1714,15 +1700,11 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A87" s="6" t="s">
+      <c r="A87" t="s">
         <v>1</v>
       </c>
-      <c r="B87" s="6"/>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="7"/>
-      <c r="F87" s="6"/>
-      <c r="G87" s="7"/>
+      <c r="E87" s="5"/>
+      <c r="G87" s="5"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
@@ -1736,16 +1718,24 @@
       <c r="G88" s="4"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A90" s="10"/>
-      <c r="B90" s="10"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="10"/>
-      <c r="G90" s="10"/>
+      <c r="A90" s="6"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="A46:G46"/>
     <mergeCell ref="A80:G80"/>
     <mergeCell ref="A85:G85"/>
     <mergeCell ref="A51:G51"/>
@@ -1753,14 +1743,6 @@
     <mergeCell ref="A63:G63"/>
     <mergeCell ref="A68:G68"/>
     <mergeCell ref="A75:G75"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A41:G41"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A15:G15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated results for MBPP with prompt 0 in 0-shot setting
</commit_message>
<xml_diff>
--- a/results/mbpp/results.xlsx
+++ b/results/mbpp/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anoop\Academics\ASU\Semester 1\CSE 576\Projects\Quirky_Quartet\results\mbpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6E0089-1DFA-4058-8EE9-30F3363E651B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B065123-A73D-4286-A569-061143A5FF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3DDA5BEF-13D0-4759-96E3-91280D99A532}"/>
   </bookViews>
@@ -189,12 +189,12 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -526,15 +526,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -660,15 +660,15 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -794,15 +794,15 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
@@ -941,15 +941,15 @@
       <c r="G22" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
@@ -978,8 +978,26 @@
       <c r="A26" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>91</v>
+      </c>
+      <c r="E26" s="5">
+        <f>B26/SUM(B26:D26)</f>
+        <v>1.9801980198019802E-2</v>
+      </c>
+      <c r="F26">
+        <v>91</v>
+      </c>
+      <c r="G26" s="5">
+        <f>F26/(SUM(B26:D26)*1)</f>
+        <v>0.90099009900990101</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
@@ -1007,15 +1025,15 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
@@ -1044,8 +1062,26 @@
       <c r="A31" t="s">
         <v>1</v>
       </c>
-      <c r="E31" s="5"/>
-      <c r="G31" s="5"/>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>17</v>
+      </c>
+      <c r="D31">
+        <v>79</v>
+      </c>
+      <c r="E31" s="5">
+        <f>B31/SUM(B31:D31)</f>
+        <v>4.9504950495049507E-2</v>
+      </c>
+      <c r="F31">
+        <v>178</v>
+      </c>
+      <c r="G31" s="5">
+        <f>F31/(SUM(B31:D31)*2)</f>
+        <v>0.88118811881188119</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
@@ -1073,15 +1109,15 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -1110,8 +1146,26 @@
       <c r="A36" t="s">
         <v>1</v>
       </c>
-      <c r="E36" s="5"/>
-      <c r="G36" s="5"/>
+      <c r="B36">
+        <v>15</v>
+      </c>
+      <c r="C36">
+        <v>29</v>
+      </c>
+      <c r="D36">
+        <v>57</v>
+      </c>
+      <c r="E36" s="5">
+        <f>B36/SUM(B36:D36)</f>
+        <v>0.14851485148514851</v>
+      </c>
+      <c r="F36">
+        <v>446</v>
+      </c>
+      <c r="G36" s="5">
+        <f>F36/(SUM(B36:D36)*5)</f>
+        <v>0.88316831683168318</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
@@ -1148,15 +1202,15 @@
       <c r="G39" s="6"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
@@ -1214,15 +1268,15 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
@@ -1280,15 +1334,15 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
@@ -1355,15 +1409,15 @@
       <c r="G56" s="6"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
@@ -1421,15 +1475,15 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
@@ -1487,15 +1541,15 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="8"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
@@ -1562,15 +1616,15 @@
       <c r="G73" s="6"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" s="8" t="s">
+      <c r="A75" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
-      <c r="F75" s="8"/>
-      <c r="G75" s="8"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
@@ -1614,15 +1668,15 @@
       <c r="G78" s="4"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" s="8" t="s">
+      <c r="A80" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B80" s="8"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
-      <c r="F80" s="8"/>
-      <c r="G80" s="8"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
@@ -1666,15 +1720,15 @@
       <c r="G83" s="4"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A85" s="8" t="s">
+      <c r="A85" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="8"/>
-      <c r="G85" s="8"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
@@ -1728,11 +1782,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A29:G29"/>
     <mergeCell ref="A34:G34"/>
     <mergeCell ref="A41:G41"/>
     <mergeCell ref="A46:G46"/>
@@ -1743,6 +1792,11 @@
     <mergeCell ref="A63:G63"/>
     <mergeCell ref="A68:G68"/>
     <mergeCell ref="A75:G75"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A29:G29"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test results for Prompt 3 pass@5
</commit_message>
<xml_diff>
--- a/results/mbpp/results.xlsx
+++ b/results/mbpp/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshit/Documents/GitHub/Quirky_Quartet/results/mbpp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA1B420-1F15-A846-BC55-1B2CC9257B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EFCE46-75E3-2F45-BD48-566C97A5A7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34940" yWindow="3880" windowWidth="25680" windowHeight="14900" xr2:uid="{3DDA5BEF-13D0-4759-96E3-91280D99A532}"/>
+    <workbookView xWindow="-36200" yWindow="660" windowWidth="25680" windowHeight="14900" xr2:uid="{3DDA5BEF-13D0-4759-96E3-91280D99A532}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="20">
   <si>
     <t>Setting</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>Prompt_id 1 - Results pass @ 2</t>
+  </si>
+  <si>
+    <t>Prompt_id 3 - Results pass @ 1</t>
+  </si>
+  <si>
+    <t>Prompt_id 3 - Results pass @ 2</t>
+  </si>
+  <si>
+    <t>Prompt_id 3 - Results pass @ 5</t>
   </si>
 </sst>
 </file>
@@ -123,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +142,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,16 +165,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -168,6 +177,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F64B8FC-649F-4A60-B32B-397739CC3A95}">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -498,25 +514,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -591,27 +607,27 @@
         <v>0.69306930693069302</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>16</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>35</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>50</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="6">
         <f t="shared" ref="E5:E6" si="0">B5/SUM(B5:D5)</f>
         <v>0.15841584158415842</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <v>50</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="6">
         <f t="shared" ref="G5:G6" si="1">F5/SUM(B5:D5)</f>
         <v>0.49504950495049505</v>
       </c>
@@ -642,15 +658,15 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -725,27 +741,27 @@
         <v>0.68316831683168322</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>24</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>51</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <v>26</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="6">
         <f t="shared" ref="E12:E13" si="2">B12/SUM(B12:D12)</f>
         <v>0.23762376237623761</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="5">
         <v>103</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="6">
         <f t="shared" ref="G12:G13" si="3">F12/(SUM(B12:D12)*2)</f>
         <v>0.50990099009900991</v>
       </c>
@@ -776,15 +792,15 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -859,27 +875,27 @@
         <v>0.65544554455445547</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="5">
         <v>38</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="5">
         <v>54</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="5">
         <v>9</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="6">
         <f t="shared" si="4"/>
         <v>0.37623762376237624</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="5">
         <v>268</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="6">
         <f t="shared" si="5"/>
         <v>0.53069306930693072</v>
       </c>
@@ -910,168 +926,429 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D22" s="6" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B27" s="5">
         <v>13</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C27" s="5">
         <v>35</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D27" s="5">
         <v>55</v>
       </c>
-      <c r="E24" s="8">
-        <f>B24/SUM(B24:D24)</f>
+      <c r="E27" s="6">
+        <f>B27/SUM(B27:D27)</f>
         <v>0.12621359223300971</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F27" s="5">
         <v>55</v>
       </c>
-      <c r="G24" s="8">
-        <f>F24/(SUM(B24:D24)*5)</f>
+      <c r="G27" s="6">
+        <f>F27/(SUM(B27:D27)*5)</f>
         <v>0.10679611650485436</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D26" s="6" t="s">
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="7">
-        <v>22</v>
-      </c>
-      <c r="C28" s="7">
-        <v>46</v>
-      </c>
-      <c r="D28" s="7">
-        <v>35</v>
-      </c>
-      <c r="E28" s="8">
-        <f>B28/SUM(B28:D28)</f>
-        <v>0.21359223300970873</v>
-      </c>
-      <c r="F28" s="7">
-        <v>115</v>
-      </c>
-      <c r="G28" s="8">
-        <f>F28/(SUM(B28:D28)*5)</f>
-        <v>0.22330097087378642</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D30" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="5">
+        <v>22</v>
+      </c>
+      <c r="C32" s="5">
+        <v>46</v>
+      </c>
+      <c r="D32" s="5">
+        <v>35</v>
+      </c>
+      <c r="E32" s="6">
+        <f>B32/SUM(B32:D32)</f>
+        <v>0.21359223300970873</v>
+      </c>
+      <c r="F32" s="5">
+        <v>115</v>
+      </c>
+      <c r="G32" s="6">
+        <f>F32/(SUM(B32:D32)*5)</f>
+        <v>0.22330097087378642</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B37" s="5">
         <v>43</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C37" s="5">
         <v>53</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D37" s="5">
         <v>7</v>
       </c>
-      <c r="E32" s="8">
-        <f>B32/SUM(B32:D32)</f>
+      <c r="E37" s="6">
+        <f>B37/SUM(B37:D37)</f>
         <v>0.41747572815533979</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F37" s="5">
         <v>274</v>
       </c>
-      <c r="G32" s="8">
-        <f>F32/(SUM(B32:D32)*5)</f>
+      <c r="G37" s="6">
+        <f>F37/(SUM(B37:D37)*5)</f>
         <v>0.53203883495145632</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D41" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="5">
+        <v>17</v>
+      </c>
+      <c r="C44" s="5">
+        <v>39</v>
+      </c>
+      <c r="D44" s="5">
+        <v>44</v>
+      </c>
+      <c r="E44" s="6">
+        <f>B44/SUM(B44:D44)</f>
+        <v>0.17</v>
+      </c>
+      <c r="F44" s="5">
+        <v>44</v>
+      </c>
+      <c r="G44" s="6">
+        <f>F44/(SUM(B44:D44)*5)</f>
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D46" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="5">
+        <v>28</v>
+      </c>
+      <c r="C49" s="5">
+        <v>51</v>
+      </c>
+      <c r="D49" s="5">
+        <v>21</v>
+      </c>
+      <c r="E49" s="6">
+        <f>B49/SUM(B49:D49)</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F49" s="5">
+        <v>88</v>
+      </c>
+      <c r="G49" s="6">
+        <f>F49/(SUM(B49:D49)*5)</f>
+        <v>0.17599999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="5">
+        <v>44</v>
+      </c>
+      <c r="C54" s="5">
+        <v>54</v>
+      </c>
+      <c r="D54" s="5">
+        <v>2</v>
+      </c>
+      <c r="E54" s="6">
+        <f>B54/(SUM(B54:D54))</f>
+        <v>0.44</v>
+      </c>
+      <c r="F54" s="5">
+        <v>229</v>
+      </c>
+      <c r="G54" s="6">
+        <f>F54/(SUM(B54:D54)*5)</f>
+        <v>0.45800000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated results for MBPP with prompt 2 in 0-shot setting
</commit_message>
<xml_diff>
--- a/results/mbpp/results.xlsx
+++ b/results/mbpp/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshit/Documents/GitHub/Quirky_Quartet/results/mbpp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anoop\Academics\ASU\Semester 1\CSE 576\Projects\Quirky_Quartet\results\mbpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EFCE46-75E3-2F45-BD48-566C97A5A7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F5EEBC-380A-4E77-A0DB-8298AEA706FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36200" yWindow="660" windowWidth="25680" windowHeight="14900" xr2:uid="{3DDA5BEF-13D0-4759-96E3-91280D99A532}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3DDA5BEF-13D0-4759-96E3-91280D99A532}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="26">
   <si>
     <t>Setting</t>
   </si>
@@ -80,22 +77,40 @@
     <t>Total Unparseable</t>
   </si>
   <si>
-    <t>Prompt_id 1 - Results pass @ 5</t>
-  </si>
-  <si>
-    <t>Prompt_id 1 - Results pass @ 1</t>
-  </si>
-  <si>
-    <t>Prompt_id 1 - Results pass @ 2</t>
-  </si>
-  <si>
-    <t>Prompt_id 3 - Results pass @ 1</t>
-  </si>
-  <si>
-    <t>Prompt_id 3 - Results pass @ 2</t>
-  </si>
-  <si>
-    <t>Prompt_id 3 - Results pass @ 5</t>
+    <t>Prompt_id 0 - Results @ 1</t>
+  </si>
+  <si>
+    <t>Prompt_id 0 - Results @ 2</t>
+  </si>
+  <si>
+    <t>Prompt_id 0 - Results @ 5</t>
+  </si>
+  <si>
+    <t>Prompt_id 1 - Results @ 1</t>
+  </si>
+  <si>
+    <t>Prompt_id 1 - Results @ 2</t>
+  </si>
+  <si>
+    <t>Prompt_id 1 - Results @ 5</t>
+  </si>
+  <si>
+    <t>Prompt_id 2 - Results @ 1</t>
+  </si>
+  <si>
+    <t>Prompt_id 2 - Results @ 2</t>
+  </si>
+  <si>
+    <t>Prompt_id 2 - Results @ 5</t>
+  </si>
+  <si>
+    <t>Prompt_id 3 - Results @ 1</t>
+  </si>
+  <si>
+    <t>Prompt_id 3 - Results @ 2</t>
+  </si>
+  <si>
+    <t>Prompt_id 3 - Results @ 5</t>
   </si>
 </sst>
 </file>
@@ -147,7 +162,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,25 +184,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -499,42 +511,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F64B8FC-649F-4A60-B32B-397739CC3A95}">
-  <dimension ref="A1:Q54"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B54" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -582,7 +584,7 @@
         <v>0.88118811881188119</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -607,32 +609,32 @@
         <v>0.69306930693069302</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>16</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>35</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>50</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <f t="shared" ref="E5:E6" si="0">B5/SUM(B5:D5)</f>
         <v>0.15841584158415842</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>50</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="4">
         <f t="shared" ref="G5:G6" si="1">F5/SUM(B5:D5)</f>
         <v>0.49504950495049505</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -657,18 +659,18 @@
         <v>0.54455445544554459</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -691,7 +693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -716,7 +718,7 @@
         <v>0.87128712871287128</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -741,32 +743,32 @@
         <v>0.68316831683168322</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="3">
         <v>24</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>51</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="3">
         <v>26</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <f t="shared" ref="E12:E13" si="2">B12/SUM(B12:D12)</f>
         <v>0.23762376237623761</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
         <v>103</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="4">
         <f t="shared" ref="G12:G13" si="3">F12/(SUM(B12:D12)*2)</f>
         <v>0.50990099009900991</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -791,18 +793,18 @@
         <v>0.54950495049504955</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -825,7 +827,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -850,7 +852,7 @@
         <v>0.84356435643564354</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -875,32 +877,32 @@
         <v>0.65544554455445547</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="3">
         <v>38</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="3">
         <v>54</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="3">
         <v>9</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="4">
         <f t="shared" si="4"/>
         <v>0.37623762376237624</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="3">
         <v>268</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="4">
         <f t="shared" si="5"/>
         <v>0.53069306930693072</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -925,27 +927,31 @@
         <v>0.51287128712871288</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -968,54 +974,68 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>91</v>
+      </c>
+      <c r="E26" s="9">
+        <f>B26/SUM(B26:D26)</f>
+        <v>1.9801980198019802E-2</v>
+      </c>
+      <c r="F26">
+        <v>91</v>
+      </c>
+      <c r="G26" s="9">
+        <f>F26/(SUM(B26:D26)*1)</f>
+        <v>0.90099009900990101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="5">
-        <v>13</v>
-      </c>
-      <c r="C27" s="5">
-        <v>35</v>
-      </c>
-      <c r="D27" s="5">
-        <v>55</v>
-      </c>
-      <c r="E27" s="6">
+      <c r="B27" s="3">
+        <v>19</v>
+      </c>
+      <c r="C27" s="3">
+        <v>32</v>
+      </c>
+      <c r="D27" s="3">
+        <v>50</v>
+      </c>
+      <c r="E27" s="4">
         <f>B27/SUM(B27:D27)</f>
-        <v>0.12621359223300971</v>
-      </c>
-      <c r="F27" s="5">
-        <v>55</v>
-      </c>
-      <c r="G27" s="6">
-        <f>F27/(SUM(B27:D27)*5)</f>
-        <v>0.10679611650485436</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29"/>
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.18811881188118812</v>
+      </c>
+      <c r="F27" s="3">
+        <v>50</v>
+      </c>
+      <c r="G27" s="4">
+        <f>F27/(SUM(B27:D27)*1)</f>
+        <v>0.49504950495049505</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -1038,54 +1058,68 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>17</v>
+      </c>
+      <c r="D31">
+        <v>79</v>
+      </c>
+      <c r="E31" s="9">
+        <f>B31/SUM(B31:D31)</f>
+        <v>4.9504950495049507E-2</v>
+      </c>
+      <c r="F31">
+        <v>178</v>
+      </c>
+      <c r="G31" s="9">
+        <f>F31/(SUM(B31:D31)*2)</f>
+        <v>0.88118811881188119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="5">
-        <v>22</v>
-      </c>
-      <c r="C32" s="5">
-        <v>46</v>
-      </c>
-      <c r="D32" s="5">
-        <v>35</v>
-      </c>
-      <c r="E32" s="6">
+      <c r="B32" s="3">
+        <v>25</v>
+      </c>
+      <c r="C32" s="3">
+        <v>49</v>
+      </c>
+      <c r="D32" s="3">
+        <v>27</v>
+      </c>
+      <c r="E32" s="4">
         <f>B32/SUM(B32:D32)</f>
-        <v>0.21359223300970873</v>
-      </c>
-      <c r="F32" s="5">
-        <v>115</v>
-      </c>
-      <c r="G32" s="6">
-        <f>F32/(SUM(B32:D32)*5)</f>
-        <v>0.22330097087378642</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.24752475247524752</v>
+      </c>
+      <c r="F32" s="3">
+        <v>105</v>
+      </c>
+      <c r="G32" s="4">
+        <f>F32/(SUM(B32:D32)*2)</f>
+        <v>0.51980198019801982</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -1108,59 +1142,77 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+      <c r="B36">
+        <v>15</v>
+      </c>
+      <c r="C36">
+        <v>29</v>
+      </c>
+      <c r="D36">
+        <v>57</v>
+      </c>
+      <c r="E36" s="9">
+        <f>B36/SUM(B36:D36)</f>
+        <v>0.14851485148514851</v>
+      </c>
+      <c r="F36">
+        <v>446</v>
+      </c>
+      <c r="G36" s="9">
+        <f>F36/(SUM(B36:D36)*5)</f>
+        <v>0.88316831683168318</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="3">
         <v>43</v>
       </c>
-      <c r="C37" s="5">
-        <v>53</v>
-      </c>
-      <c r="D37" s="5">
+      <c r="C37" s="3">
+        <v>51</v>
+      </c>
+      <c r="D37" s="3">
         <v>7</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="4">
         <f>B37/SUM(B37:D37)</f>
-        <v>0.41747572815533979</v>
-      </c>
-      <c r="F37" s="5">
-        <v>274</v>
-      </c>
-      <c r="G37" s="6">
+        <v>0.42574257425742573</v>
+      </c>
+      <c r="F37" s="3">
+        <v>259</v>
+      </c>
+      <c r="G37" s="4">
         <f>F37/(SUM(B37:D37)*5)</f>
-        <v>0.53203883495145632</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D41" s="4" t="s">
+        <v>0.51287128712871288</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -1183,50 +1235,50 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+      <c r="E43" s="9"/>
+      <c r="G43" s="9"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B44" s="5">
-        <v>17</v>
-      </c>
-      <c r="C44" s="5">
-        <v>39</v>
-      </c>
-      <c r="D44" s="5">
-        <v>44</v>
-      </c>
-      <c r="E44" s="6">
+      <c r="B44" s="3">
+        <v>13</v>
+      </c>
+      <c r="C44" s="3">
+        <v>35</v>
+      </c>
+      <c r="D44" s="3">
+        <v>55</v>
+      </c>
+      <c r="E44" s="4">
         <f>B44/SUM(B44:D44)</f>
-        <v>0.17</v>
-      </c>
-      <c r="F44" s="5">
-        <v>44</v>
-      </c>
-      <c r="G44" s="6">
-        <f>F44/(SUM(B44:D44)*5)</f>
-        <v>8.7999999999999995E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D46" s="4" t="s">
+        <v>0.12621359223300971</v>
+      </c>
+      <c r="F44" s="3">
+        <v>55</v>
+      </c>
+      <c r="G44" s="4">
+        <f>F44/(SUM(B44:D44)*1)</f>
+        <v>0.53398058252427183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -1249,50 +1301,50 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="5" t="s">
+      <c r="E48" s="9"/>
+      <c r="G48" s="9"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B49" s="5">
-        <v>28</v>
-      </c>
-      <c r="C49" s="5">
-        <v>51</v>
-      </c>
-      <c r="D49" s="5">
-        <v>21</v>
-      </c>
-      <c r="E49" s="6">
+      <c r="B49" s="3">
+        <v>22</v>
+      </c>
+      <c r="C49" s="3">
+        <v>46</v>
+      </c>
+      <c r="D49" s="3">
+        <v>35</v>
+      </c>
+      <c r="E49" s="4">
         <f>B49/SUM(B49:D49)</f>
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="F49" s="5">
-        <v>88</v>
-      </c>
-      <c r="G49" s="6">
-        <f>F49/(SUM(B49:D49)*5)</f>
-        <v>0.17599999999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D51" s="4" t="s">
+        <v>0.21359223300970873</v>
+      </c>
+      <c r="F49" s="3">
+        <v>115</v>
+      </c>
+      <c r="G49" s="4">
+        <f>F49/(SUM(B49:D49)*2)</f>
+        <v>0.55825242718446599</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -1315,46 +1367,529 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
+      <c r="E53" s="9"/>
+      <c r="G53" s="9"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B54" s="3">
+        <v>43</v>
+      </c>
+      <c r="C54" s="3">
+        <v>53</v>
+      </c>
+      <c r="D54" s="3">
+        <v>7</v>
+      </c>
+      <c r="E54" s="4">
+        <f>B54/SUM(B54:D54)</f>
+        <v>0.41747572815533979</v>
+      </c>
+      <c r="F54" s="3">
+        <v>274</v>
+      </c>
+      <c r="G54" s="4">
+        <f>F54/(SUM(B54:D54)*5)</f>
+        <v>0.53203883495145632</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>6</v>
+      </c>
+      <c r="D60">
+        <v>91</v>
+      </c>
+      <c r="E60" s="9">
+        <f>B60/SUM(B60:D60)</f>
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>91</v>
+      </c>
+      <c r="G60" s="9">
+        <f>F60/(SUM(B60:D60)*1)</f>
+        <v>0.93814432989690721</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="3">
+        <v>15</v>
+      </c>
+      <c r="C61" s="3">
+        <v>30</v>
+      </c>
+      <c r="D61" s="3">
+        <v>56</v>
+      </c>
+      <c r="E61" s="4">
+        <f>B61/SUM(B61:D61)</f>
+        <v>0.14851485148514851</v>
+      </c>
+      <c r="F61" s="3">
+        <v>56</v>
+      </c>
+      <c r="G61" s="4">
+        <f>F61/(SUM(B61:D61)*1)</f>
+        <v>0.5544554455445545</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65">
+        <v>10</v>
+      </c>
+      <c r="D65">
+        <v>89</v>
+      </c>
+      <c r="E65" s="9">
+        <f>B65/SUM(B65:D65)</f>
+        <v>1.9801980198019802E-2</v>
+      </c>
+      <c r="F65">
+        <v>189</v>
+      </c>
+      <c r="G65" s="9">
+        <f>F65/(SUM(B65:D65)*2)</f>
+        <v>0.9356435643564357</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="3">
+        <v>26</v>
+      </c>
+      <c r="C66" s="3">
+        <v>47</v>
+      </c>
+      <c r="D66" s="3">
+        <v>28</v>
+      </c>
+      <c r="E66" s="4">
+        <f>B66/SUM(B66:D66)</f>
+        <v>0.25742574257425743</v>
+      </c>
+      <c r="F66" s="3">
+        <v>114</v>
+      </c>
+      <c r="G66" s="4">
+        <f>F66/(SUM(B66:D66)*2)</f>
+        <v>0.5643564356435643</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <v>4</v>
+      </c>
+      <c r="C70">
+        <v>25</v>
+      </c>
+      <c r="D70">
+        <v>72</v>
+      </c>
+      <c r="E70" s="9">
+        <f>B70/SUM(B70:D70)</f>
+        <v>3.9603960396039604E-2</v>
+      </c>
+      <c r="F70">
+        <v>474</v>
+      </c>
+      <c r="G70" s="9">
+        <f>F70/(SUM(B70:D70)*5)</f>
+        <v>0.93861386138613856</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A71" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" s="3">
         <v>44</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C71" s="3">
         <v>54</v>
       </c>
-      <c r="D54" s="5">
+      <c r="D71" s="3">
+        <v>3</v>
+      </c>
+      <c r="E71" s="4">
+        <f>B71/SUM(B71:D71)</f>
+        <v>0.43564356435643564</v>
+      </c>
+      <c r="F71" s="3">
+        <v>258</v>
+      </c>
+      <c r="G71" s="4">
+        <f>F71/(SUM(B71:D71)*5)</f>
+        <v>0.5108910891089109</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A73" s="6"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="8"/>
+      <c r="G75" s="8"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>1</v>
+      </c>
+      <c r="E77" s="9"/>
+      <c r="G77" s="9"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A78" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" s="3">
+        <v>17</v>
+      </c>
+      <c r="C78" s="3">
+        <v>39</v>
+      </c>
+      <c r="D78" s="3">
+        <v>44</v>
+      </c>
+      <c r="E78" s="4">
+        <f>B78/SUM(B78:D78)</f>
+        <v>0.17</v>
+      </c>
+      <c r="F78" s="3">
+        <v>44</v>
+      </c>
+      <c r="G78" s="4">
+        <f>F78/(SUM(B78:D78)*1)</f>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+      <c r="G80" s="8"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>1</v>
+      </c>
+      <c r="E82" s="9"/>
+      <c r="G82" s="9"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" s="3">
+        <v>28</v>
+      </c>
+      <c r="C83" s="3">
+        <v>51</v>
+      </c>
+      <c r="D83" s="3">
+        <v>21</v>
+      </c>
+      <c r="E83" s="4">
+        <f>B83/SUM(B83:D83)</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F83" s="3">
+        <v>88</v>
+      </c>
+      <c r="G83" s="4">
+        <f>F83/(SUM(B83:D83)*2)</f>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>1</v>
+      </c>
+      <c r="E87" s="9"/>
+      <c r="G87" s="9"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" s="3">
+        <v>44</v>
+      </c>
+      <c r="C88" s="3">
+        <v>54</v>
+      </c>
+      <c r="D88" s="3">
         <v>2</v>
       </c>
-      <c r="E54" s="6">
-        <f>B54/(SUM(B54:D54))</f>
+      <c r="E88" s="4">
+        <f>B88/(SUM(B88:D88))</f>
         <v>0.44</v>
       </c>
-      <c r="F54" s="5">
+      <c r="F88" s="3">
         <v>229</v>
       </c>
-      <c r="G54" s="6">
-        <f>F54/(SUM(B54:D54)*5)</f>
+      <c r="G88" s="4">
+        <f>F88/(SUM(B88:D88)*5)</f>
         <v>0.45800000000000002</v>
       </c>
     </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="6"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:Q1"/>
+  <mergeCells count="15">
+    <mergeCell ref="A80:G80"/>
+    <mergeCell ref="A85:G85"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="A58:G58"/>
+    <mergeCell ref="A63:G63"/>
+    <mergeCell ref="A68:G68"/>
+    <mergeCell ref="A75:G75"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="A46:G46"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A15:G15"/>

</xml_diff>

<commit_message>
results for prompt1 0-shot
</commit_message>
<xml_diff>
--- a/results/mbpp/results.xlsx
+++ b/results/mbpp/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anoop\Academics\ASU\Semester 1\CSE 576\Projects\Quirky_Quartet\results\mbpp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshit/Documents/GitHub/Quirky_Quartet/results/mbpp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F5EEBC-380A-4E77-A0DB-8298AEA706FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048C5228-836E-B943-810D-49D3A0960C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3DDA5BEF-13D0-4759-96E3-91280D99A532}"/>
+    <workbookView xWindow="-36100" yWindow="1680" windowWidth="16420" windowHeight="14620" xr2:uid="{3DDA5BEF-13D0-4759-96E3-91280D99A532}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -186,20 +189,20 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -513,30 +516,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F64B8FC-649F-4A60-B32B-397739CC3A95}">
   <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B54" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -584,7 +587,7 @@
         <v>0.88118811881188119</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -609,7 +612,7 @@
         <v>0.69306930693069302</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -634,7 +637,7 @@
         <v>0.49504950495049505</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -659,18 +662,18 @@
         <v>0.54455445544554459</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -718,7 +721,7 @@
         <v>0.87128712871287128</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -743,7 +746,7 @@
         <v>0.68316831683168322</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -768,7 +771,7 @@
         <v>0.50990099009900991</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -793,18 +796,18 @@
         <v>0.54950495049504955</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -827,7 +830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -852,7 +855,7 @@
         <v>0.84356435643564354</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -877,7 +880,7 @@
         <v>0.65544554455445547</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
@@ -902,7 +905,7 @@
         <v>0.53069306930693072</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -927,20 +930,20 @@
         <v>0.51287128712871288</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>14</v>
       </c>
@@ -951,7 +954,7 @@
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -974,7 +977,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -987,19 +990,19 @@
       <c r="D26">
         <v>91</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="7">
         <f>B26/SUM(B26:D26)</f>
         <v>1.9801980198019802E-2</v>
       </c>
       <c r="F26">
         <v>91</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="7">
         <f>F26/(SUM(B26:D26)*1)</f>
         <v>0.90099009900990101</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>3</v>
       </c>
@@ -1024,7 +1027,7 @@
         <v>0.49504950495049505</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>15</v>
       </c>
@@ -1035,7 +1038,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -1071,19 +1074,19 @@
       <c r="D31">
         <v>79</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="7">
         <f>B31/SUM(B31:D31)</f>
         <v>4.9504950495049507E-2</v>
       </c>
       <c r="F31">
         <v>178</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="7">
         <f>F31/(SUM(B31:D31)*2)</f>
         <v>0.88118811881188119</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>3</v>
       </c>
@@ -1108,7 +1111,7 @@
         <v>0.51980198019801982</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>16</v>
       </c>
@@ -1119,7 +1122,7 @@
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -1142,7 +1145,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -1155,19 +1158,19 @@
       <c r="D36">
         <v>57</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="7">
         <f>B36/SUM(B36:D36)</f>
         <v>0.14851485148514851</v>
       </c>
       <c r="F36">
         <v>446</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="7">
         <f>F36/(SUM(B36:D36)*5)</f>
         <v>0.88316831683168318</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>3</v>
       </c>
@@ -1192,16 +1195,16 @@
         <v>0.51287128712871288</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>17</v>
       </c>
@@ -1212,7 +1215,7 @@
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -1235,14 +1238,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>1</v>
       </c>
-      <c r="E43" s="9"/>
-      <c r="G43" s="9"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E43" s="7"/>
+      <c r="G43" s="7"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>3</v>
       </c>
@@ -1267,7 +1270,7 @@
         <v>0.53398058252427183</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>18</v>
       </c>
@@ -1278,7 +1281,7 @@
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -1301,14 +1304,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>1</v>
       </c>
-      <c r="E48" s="9"/>
-      <c r="G48" s="9"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E48" s="7"/>
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>3</v>
       </c>
@@ -1333,7 +1336,7 @@
         <v>0.55825242718446599</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>19</v>
       </c>
@@ -1344,7 +1347,7 @@
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -1367,14 +1370,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>1</v>
       </c>
-      <c r="E53" s="9"/>
-      <c r="G53" s="9"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E53" s="7"/>
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>3</v>
       </c>
@@ -1399,16 +1402,16 @@
         <v>0.53203883495145632</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
         <v>20</v>
       </c>
@@ -1419,7 +1422,7 @@
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
@@ -1442,7 +1445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>1</v>
       </c>
@@ -1455,19 +1458,19 @@
       <c r="D60">
         <v>91</v>
       </c>
-      <c r="E60" s="9">
+      <c r="E60" s="7">
         <f>B60/SUM(B60:D60)</f>
         <v>0</v>
       </c>
       <c r="F60">
         <v>91</v>
       </c>
-      <c r="G60" s="9">
+      <c r="G60" s="7">
         <f>F60/(SUM(B60:D60)*1)</f>
         <v>0.93814432989690721</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>3</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>0.5544554455445545</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
         <v>21</v>
       </c>
@@ -1503,7 +1506,7 @@
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +1529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>1</v>
       </c>
@@ -1539,19 +1542,19 @@
       <c r="D65">
         <v>89</v>
       </c>
-      <c r="E65" s="9">
+      <c r="E65" s="7">
         <f>B65/SUM(B65:D65)</f>
         <v>1.9801980198019802E-2</v>
       </c>
       <c r="F65">
         <v>189</v>
       </c>
-      <c r="G65" s="9">
+      <c r="G65" s="7">
         <f>F65/(SUM(B65:D65)*2)</f>
         <v>0.9356435643564357</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>3</v>
       </c>
@@ -1576,7 +1579,7 @@
         <v>0.5643564356435643</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
         <v>22</v>
       </c>
@@ -1587,7 +1590,7 @@
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
@@ -1610,7 +1613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>1</v>
       </c>
@@ -1623,19 +1626,19 @@
       <c r="D70">
         <v>72</v>
       </c>
-      <c r="E70" s="9">
+      <c r="E70" s="7">
         <f>B70/SUM(B70:D70)</f>
         <v>3.9603960396039604E-2</v>
       </c>
       <c r="F70">
         <v>474</v>
       </c>
-      <c r="G70" s="9">
+      <c r="G70" s="7">
         <f>F70/(SUM(B70:D70)*5)</f>
         <v>0.93861386138613856</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>3</v>
       </c>
@@ -1660,16 +1663,16 @@
         <v>0.5108910891089109</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73" s="6"/>
-      <c r="B73" s="6"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
-      <c r="G73" s="6"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
         <v>23</v>
       </c>
@@ -1680,7 +1683,7 @@
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
@@ -1703,14 +1706,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>1</v>
       </c>
-      <c r="E77" s="9"/>
-      <c r="G77" s="9"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>11</v>
+      </c>
+      <c r="D77">
+        <v>93</v>
+      </c>
+      <c r="E77" s="7">
+        <v>9.5200000000000007E-3</v>
+      </c>
+      <c r="F77">
+        <v>93</v>
+      </c>
+      <c r="G77" s="7">
+        <v>0.88571</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>3</v>
       </c>
@@ -1735,7 +1754,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="8" t="s">
         <v>24</v>
       </c>
@@ -1746,7 +1765,7 @@
       <c r="F80" s="8"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>0</v>
       </c>
@@ -1769,14 +1788,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>1</v>
       </c>
-      <c r="E82" s="9"/>
-      <c r="G82" s="9"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B82">
+        <v>6</v>
+      </c>
+      <c r="C82">
+        <v>14</v>
+      </c>
+      <c r="D82">
+        <v>85</v>
+      </c>
+      <c r="E82" s="7">
+        <v>5.7140000000000003E-2</v>
+      </c>
+      <c r="F82">
+        <v>189</v>
+      </c>
+      <c r="G82" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>3</v>
       </c>
@@ -1801,7 +1836,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
         <v>25</v>
       </c>
@@ -1812,7 +1847,7 @@
       <c r="F85" s="8"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>0</v>
       </c>
@@ -1835,14 +1870,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>1</v>
       </c>
-      <c r="E87" s="9"/>
-      <c r="G87" s="9"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B87">
+        <v>10</v>
+      </c>
+      <c r="C87">
+        <v>23</v>
+      </c>
+      <c r="D87">
+        <v>72</v>
+      </c>
+      <c r="E87" s="7">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="F87">
+        <v>480</v>
+      </c>
+      <c r="G87" s="7">
+        <v>0.91429000000000005</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>3</v>
       </c>
@@ -1867,17 +1918,25 @@
         <v>0.45800000000000002</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A90" s="6"/>
-      <c r="B90" s="6"/>
-      <c r="C90" s="6"/>
-      <c r="D90" s="6"/>
-      <c r="E90" s="6"/>
-      <c r="F90" s="6"/>
-      <c r="G90" s="6"/>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="A46:G46"/>
     <mergeCell ref="A80:G80"/>
     <mergeCell ref="A85:G85"/>
     <mergeCell ref="A51:G51"/>
@@ -1885,14 +1944,6 @@
     <mergeCell ref="A63:G63"/>
     <mergeCell ref="A68:G68"/>
     <mergeCell ref="A75:G75"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A41:G41"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A15:G15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated results for Prompt 1 0-shot
</commit_message>
<xml_diff>
--- a/results/mbpp/results.xlsx
+++ b/results/mbpp/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshit/Documents/GitHub/Quirky_Quartet/results/mbpp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048C5228-836E-B943-810D-49D3A0960C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D7DFF2-9137-3947-9B8D-BD063AED8CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36100" yWindow="1680" windowWidth="16420" windowHeight="14620" xr2:uid="{3DDA5BEF-13D0-4759-96E3-91280D99A532}"/>
   </bookViews>
@@ -192,12 +192,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F64B8FC-649F-4A60-B32B-397739CC3A95}">
   <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -529,15 +529,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -663,15 +663,15 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -797,15 +797,15 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -944,15 +944,15 @@
       <c r="G22" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -1028,15 +1028,15 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
@@ -1112,15 +1112,15 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -1205,15 +1205,15 @@
       <c r="G39" s="5"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
@@ -1242,8 +1242,24 @@
       <c r="A43" t="s">
         <v>1</v>
       </c>
-      <c r="E43" s="7"/>
-      <c r="G43" s="7"/>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>101</v>
+      </c>
+      <c r="E43" s="7">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>101</v>
+      </c>
+      <c r="G43" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
@@ -1271,15 +1287,15 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
@@ -1308,8 +1324,24 @@
       <c r="A48" t="s">
         <v>1</v>
       </c>
-      <c r="E48" s="7"/>
-      <c r="G48" s="7"/>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>99</v>
+      </c>
+      <c r="E48" s="7">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>200</v>
+      </c>
+      <c r="G48" s="7">
+        <v>0.99009999999999998</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
@@ -1337,15 +1369,15 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
@@ -1374,8 +1406,24 @@
       <c r="A53" t="s">
         <v>1</v>
       </c>
-      <c r="E53" s="7"/>
-      <c r="G53" s="7"/>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>97</v>
+      </c>
+      <c r="E53" s="7">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="F53">
+        <v>499</v>
+      </c>
+      <c r="G53" s="7">
+        <v>0.98812</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
@@ -1412,15 +1460,15 @@
       <c r="G56" s="5"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
@@ -1496,15 +1544,15 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
@@ -1580,15 +1628,15 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="8"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
@@ -1673,15 +1721,15 @@
       <c r="G73" s="5"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="8" t="s">
+      <c r="A75" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
-      <c r="F75" s="8"/>
-      <c r="G75" s="8"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
@@ -1755,15 +1803,15 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A80" s="8" t="s">
+      <c r="A80" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B80" s="8"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
-      <c r="F80" s="8"/>
-      <c r="G80" s="8"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
@@ -1837,15 +1885,15 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="8" t="s">
+      <c r="A85" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="8"/>
-      <c r="G85" s="8"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
@@ -1929,11 +1977,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A29:G29"/>
     <mergeCell ref="A34:G34"/>
     <mergeCell ref="A41:G41"/>
     <mergeCell ref="A46:G46"/>
@@ -1944,6 +1987,11 @@
     <mergeCell ref="A63:G63"/>
     <mergeCell ref="A68:G68"/>
     <mergeCell ref="A75:G75"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A29:G29"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>